<commit_message>
Better dialogue system logic
</commit_message>
<xml_diff>
--- a/Assets/Resources/ScriptableObjects/Tutorial/Excel/TutorialLines.xlsx
+++ b/Assets/Resources/ScriptableObjects/Tutorial/Excel/TutorialLines.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="11">
   <si>
     <t>ID</t>
   </si>
@@ -38,6 +38,12 @@
     <t>Line</t>
   </si>
   <si>
+    <t>PanelID</t>
+  </si>
+  <si>
+    <t>PanelPosition</t>
+  </si>
+  <si>
     <t>error</t>
   </si>
   <si>
@@ -46,6 +52,9 @@
   <si>
     <t>江承彦是一名&lt;color=#FF0000&gt;魁梧男子&lt;/color&gt;。
 江承彦是双开门大冰箱。</t>
+  </si>
+  <si>
+    <t>下</t>
   </si>
   <si>
     <t>懒惰病毒</t>
@@ -64,10 +73,16 @@
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
-  <fonts count="20">
+  <fonts count="21">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <name val="宋体"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -537,141 +552,144 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="6" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1">
@@ -991,19 +1009,20 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:C28"/>
+  <dimension ref="A1:E28"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelCol="2"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelCol="4"/>
   <cols>
     <col min="2" max="2" width="19.8727272727273" customWidth="1"/>
-    <col min="3" max="3" width="98.4909090909091" customWidth="1"/>
+    <col min="3" max="3" width="70.4727272727273" customWidth="1"/>
+    <col min="5" max="5" width="17.9272727272727" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:5">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1013,38 +1032,50 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
+      <c r="D1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="2" spans="1:3">
-      <c r="A2" s="2">
+      <c r="A2" s="3">
         <v>0</v>
       </c>
-      <c r="B2" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="3" ht="28" spans="1:3">
+      <c r="B2" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" ht="28" spans="1:5">
       <c r="A3">
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3">
+        <v>6</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
       <c r="A4">
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="C4" t="s">
-        <v>7</v>
+        <v>10</v>
+      </c>
+      <c r="E4" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="5" spans="1:1">

</xml_diff>

<commit_message>
Level Index starts from zero……
</commit_message>
<xml_diff>
--- a/Assets/Resources/ScriptableObjects/Tutorial/Excel/TutorialLines.xlsx
+++ b/Assets/Resources/ScriptableObjects/Tutorial/Excel/TutorialLines.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\UnityProjects\Slay-the-Virus-2\Assets\Resources\ScriptableObjects\Tutorial\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D4CF31B-379B-44BF-8585-F5BF85145638}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1603FC6C-0963-479A-ABE0-2AFC20C0D6CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -599,8 +599,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H48"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="E31" sqref="E31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Card Remake Part III
</commit_message>
<xml_diff>
--- a/Assets/Resources/ScriptableObjects/Tutorial/Excel/TutorialLines.xlsx
+++ b/Assets/Resources/ScriptableObjects/Tutorial/Excel/TutorialLines.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\UnityProjects\Slay-the-Virus-2\Assets\Resources\ScriptableObjects\Tutorial\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51EA1479-C41E-428E-9A3E-6C44596F9AA3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9EA36108-823A-4856-BBD9-52A727DDB4B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="105">
   <si>
     <t>ID</t>
   </si>
@@ -774,8 +774,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H115"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A88" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="D100" sqref="D100"/>
+    <sheetView tabSelected="1" topLeftCell="A49" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="D66" sqref="D66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" x14ac:dyDescent="0.25"/>
@@ -1454,9 +1454,6 @@
       <c r="A55">
         <v>53</v>
       </c>
-      <c r="B55" t="s">
-        <v>51</v>
-      </c>
       <c r="C55" t="s">
         <v>9</v>
       </c>

</xml_diff>